<commit_message>
Fix a cell with the wrong format
</commit_message>
<xml_diff>
--- a/CA7_Process_Documents/Project timeline.xlsx
+++ b/CA7_Process_Documents/Project timeline.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D895B286-623E-4455-909F-4A7EF155B281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Project Timeline" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Project Timeline'!$A$1:$L$14</definedName>
     <definedName name="ProjectEnd">INDEX(ProjectDetails[],MIN(ROW(data))+ROWS(data)-1,1)</definedName>
     <definedName name="ProjectStart">ProjectDetails[]('Project Timeline'!$B$17)</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Project Timeline'!$A$1:$L$14</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -102,7 +101,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
@@ -389,18 +388,18 @@
     </xf>
   </cellXfs>
   <cellStyles count="12">
-    <cellStyle name="Bemærk!" xfId="11" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Komma" xfId="6" builtinId="3" customBuiltin="1"/>
-    <cellStyle name="Komma [0]" xfId="7" builtinId="6" customBuiltin="1"/>
+    <cellStyle name="Comma" xfId="6" builtinId="3" customBuiltin="1"/>
+    <cellStyle name="Comma [0]" xfId="7" builtinId="6" customBuiltin="1"/>
+    <cellStyle name="Currency" xfId="8" builtinId="4" customBuiltin="1"/>
+    <cellStyle name="Currency [0]" xfId="9" builtinId="7" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Overskrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Overskrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Overskrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Overskrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Procent" xfId="10" builtinId="5" customBuiltin="1"/>
-    <cellStyle name="Titel" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Valuta" xfId="8" builtinId="4" customBuiltin="1"/>
-    <cellStyle name="Valuta [0]" xfId="9" builtinId="7" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="11" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="10" builtinId="5" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -468,7 +467,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Project Timeline" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Project Timeline" pivot="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="Project Timeline" pivot="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="5"/>
       <tableStyleElement type="headerRow" dxfId="4"/>
     </tableStyle>
@@ -487,7 +486,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="da-DK"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -554,7 +553,7 @@
                     <a:fld id="{38BBA013-30A3-4E6C-A1D3-5EF6D1513EB1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CELLEOMRÅDE]</a:t>
+                      <a:t>[CELLRANGE]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" baseline="0"/>
                   </a:p>
@@ -562,9 +561,9 @@
                     <a:fld id="{695A9D1D-15EE-425F-A650-75662AB74DA2}" type="CATEGORYNAME">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[KATEGORINAVN]</a:t>
+                      <a:t>[CATEGORY NAME]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="da-DK"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -579,6 +578,7 @@
 </c:separator>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -603,7 +603,7 @@
                     <a:fld id="{3AEDABC0-ED0B-4B29-B966-F0824DBF65DE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CELLEOMRÅDE]</a:t>
+                      <a:t>[CELLRANGE]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" baseline="0"/>
                   </a:p>
@@ -611,9 +611,9 @@
                     <a:fld id="{8ADBBBA2-1DBF-4F21-A72E-E068DE7E37C1}" type="CATEGORYNAME">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[KATEGORINAVN]</a:t>
+                      <a:t>[CATEGORY NAME]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="da-DK"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -628,6 +628,7 @@
 </c:separator>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -652,7 +653,7 @@
                     <a:fld id="{89C66AAD-5390-4101-A161-865A928CC1AE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CELLEOMRÅDE]</a:t>
+                      <a:t>[CELLRANGE]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" baseline="0"/>
                   </a:p>
@@ -660,9 +661,9 @@
                     <a:fld id="{EFC92BFA-4E62-46E3-9E76-D1EBE8419B53}" type="CATEGORYNAME">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[KATEGORINAVN]</a:t>
+                      <a:t>[CATEGORY NAME]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="da-DK"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -677,6 +678,7 @@
 </c:separator>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -701,7 +703,7 @@
                     <a:fld id="{EF4A7E30-7AF8-4233-B90F-4C5786D1B879}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CELLEOMRÅDE]</a:t>
+                      <a:t>[CELLRANGE]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" baseline="0"/>
                   </a:p>
@@ -709,9 +711,9 @@
                     <a:fld id="{BA519C51-CDAD-4385-B9A0-6D3A04256C2F}" type="CATEGORYNAME">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[KATEGORINAVN]</a:t>
+                      <a:t>[CATEGORY NAME]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="da-DK"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -726,6 +728,7 @@
 </c:separator>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -750,7 +753,7 @@
                     <a:fld id="{41AC6839-2D7B-4CE5-BC64-BDE049CAC51D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CELLEOMRÅDE]</a:t>
+                      <a:t>[CELLRANGE]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" baseline="0"/>
                   </a:p>
@@ -758,9 +761,9 @@
                     <a:fld id="{37131ACD-84F4-42EB-814F-3CBCFA9F05AF}" type="CATEGORYNAME">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[KATEGORINAVN]</a:t>
+                      <a:t>[CATEGORY NAME]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="da-DK"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -775,6 +778,7 @@
 </c:separator>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -799,7 +803,7 @@
                     <a:fld id="{CE72315B-35BD-4F85-A731-B5509EE2FDF0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CELLEOMRÅDE]</a:t>
+                      <a:t>[CELLRANGE]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" baseline="0"/>
                   </a:p>
@@ -807,9 +811,9 @@
                     <a:fld id="{A55CB0EC-89B2-467B-85A1-0549DB7653E7}" type="CATEGORYNAME">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[KATEGORINAVN]</a:t>
+                      <a:t>[CATEGORY NAME]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="da-DK"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -824,6 +828,7 @@
 </c:separator>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -848,7 +853,7 @@
                     <a:fld id="{F1682120-E413-489F-BBFC-DA651141CB86}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CELLEOMRÅDE]</a:t>
+                      <a:t>[CELLRANGE]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" baseline="0"/>
                   </a:p>
@@ -856,9 +861,9 @@
                     <a:fld id="{DF5C3B40-E92F-4EB1-808D-51167C502D28}" type="CATEGORYNAME">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[KATEGORINAVN]</a:t>
+                      <a:t>[CATEGORY NAME]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="da-DK"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -873,6 +878,7 @@
 </c:separator>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -897,7 +903,7 @@
                     <a:fld id="{9100B6D6-BCD7-4526-B0FA-27C34E1F9D33}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CELLEOMRÅDE]</a:t>
+                      <a:t>[CELLRANGE]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" baseline="0"/>
                   </a:p>
@@ -905,9 +911,9 @@
                     <a:fld id="{63F6FEE7-E7B9-47A4-AD99-F858ED888535}" type="CATEGORYNAME">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[KATEGORINAVN]</a:t>
+                      <a:t>[CATEGORY NAME]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="da-DK"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -922,6 +928,7 @@
 </c:separator>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -946,7 +953,7 @@
                     <a:fld id="{3385B721-571E-4BBB-A385-E771BDC53DC7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CELLEOMRÅDE]</a:t>
+                      <a:t>[CELLRANGE]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" baseline="0"/>
                   </a:p>
@@ -954,9 +961,9 @@
                     <a:fld id="{266135CB-479F-4905-A553-8B3EA861FA68}" type="CATEGORYNAME">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[KATEGORINAVN]</a:t>
+                      <a:t>[CATEGORY NAME]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="da-DK"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -971,6 +978,7 @@
 </c:separator>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -995,7 +1003,7 @@
                     <a:fld id="{70EBAD28-6B3E-4AD0-BE0D-03059317BF5A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CELLEOMRÅDE]</a:t>
+                      <a:t>[CELLRANGE]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" baseline="0"/>
                   </a:p>
@@ -1003,9 +1011,9 @@
                     <a:fld id="{E2100826-A16D-4679-AF10-D241A3D148C0}" type="CATEGORYNAME">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[KATEGORINAVN]</a:t>
+                      <a:t>[CATEGORY NAME]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="da-DK"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1020,6 +1028,7 @@
 </c:separator>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -1044,7 +1053,7 @@
                     <a:fld id="{AE0859E4-BF7E-44F5-AA70-6251FE00BDB3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CELLEOMRÅDE]</a:t>
+                      <a:t>[CELLRANGE]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" baseline="0"/>
                   </a:p>
@@ -1052,9 +1061,9 @@
                     <a:fld id="{0617D681-6427-422C-86DC-EE73622515E9}" type="CATEGORYNAME">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[KATEGORINAVN]</a:t>
+                      <a:t>[CATEGORY NAME]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="da-DK"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1069,6 +1078,7 @@
 </c:separator>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -1093,7 +1103,7 @@
                     <a:fld id="{85C1A84E-729C-4046-8960-A8CB5BD2C35F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CELLEOMRÅDE]</a:t>
+                      <a:t>[CELLRANGE]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" baseline="0"/>
                   </a:p>
@@ -1101,9 +1111,9 @@
                     <a:fld id="{0D95E02C-930F-4864-9E58-3980F3EDDDF4}" type="CATEGORYNAME">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[KATEGORINAVN]</a:t>
+                      <a:t>[CATEGORY NAME]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="da-DK"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1118,6 +1128,7 @@
 </c:separator>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -1142,7 +1153,7 @@
                     <a:fld id="{6765A073-0BC3-43F1-944D-00DF9C4FC898}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[CELLEOMRÅDE]</a:t>
+                      <a:t>[CELLRANGE]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" baseline="0"/>
                   </a:p>
@@ -1150,9 +1161,9 @@
                     <a:fld id="{4DCF4CA1-F86D-4829-92FB-8AD8358ACA12}" type="CATEGORYNAME">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[KATEGORINAVN]</a:t>
+                      <a:t>[CATEGORY NAME]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="da-DK"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1196,7 +1207,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="da-DK"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -1459,7 +1470,7 @@
                 <c:pt idx="6">
                   <c:v>44529</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="m/d/yyyy">
+                <c:pt idx="7">
                   <c:v>44538</c:v>
                 </c:pt>
                 <c:pt idx="8">
@@ -1581,7 +1592,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="da-DK"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="717044496"/>
@@ -1674,7 +1685,7 @@
           </a:solidFill>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="da-DK"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2173,16 +2184,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="ProjectDetails" displayName="ProjectDetails" ref="B16:F29" totalsRowShown="0" headerRowDxfId="3">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B17:F30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="ProjectDetails" displayName="ProjectDetails" ref="B16:F29" totalsRowShown="0" headerRowDxfId="3">
+  <sortState ref="B17:F30">
     <sortCondition ref="B21"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Milestone" dataDxfId="1" dataCellStyle="Normal"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Assigned To" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Position" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Baseline">
+    <tableColumn id="1" name="Date" dataDxfId="2"/>
+    <tableColumn id="2" name="Milestone" dataDxfId="1" dataCellStyle="Normal"/>
+    <tableColumn id="6" name="Assigned To" dataCellStyle="Normal"/>
+    <tableColumn id="4" name="Position" dataDxfId="0"/>
+    <tableColumn id="5" name="Baseline">
       <calculatedColumnFormula>0</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2457,15 +2468,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2858,7 +2869,7 @@
       <c r="L23" s="19"/>
     </row>
     <row r="24" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="31">
+      <c r="B24" s="13">
         <v>44538</v>
       </c>
       <c r="C24" s="30" t="s">
@@ -2973,14 +2984,14 @@
     <mergeCell ref="B2:L14"/>
   </mergeCells>
   <dataValidations count="8">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create a Project Timeline with Milestones in this worksheet. Enter details in Project Details table. Chart is in cell B2 and Tip is in cell H17" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell. Line chart showing each milestone on the corresponding timeframe is in cell below" sqref="B1:C1" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter project details in table below" sqref="B15" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Date in this column under this heading" sqref="B16" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Milestone in this column under this heading" sqref="C16" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Assigned To name in this column under this heading" sqref="D16" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter chart Position in this column under this heading. Project Timeline Tip is in cell at right" sqref="E16" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Project Timeline Tip is in cell below" sqref="H16:I16" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create a Project Timeline with Milestones in this worksheet. Enter details in Project Details table. Chart is in cell B2 and Tip is in cell H17" sqref="A1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell. Line chart showing each milestone on the corresponding timeframe is in cell below" sqref="B1:C1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter project details in table below" sqref="B15"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Date in this column under this heading" sqref="B16"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Milestone in this column under this heading" sqref="C16"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Assigned To name in this column under this heading" sqref="D16"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter chart Position in this column under this heading. Project Timeline Tip is in cell at right" sqref="E16"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Project Timeline Tip is in cell below" sqref="H16:I16"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2996,23 +3007,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9677210f24a1be23c92c90fd886aa0aa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="60e05723c5c1908df1a1a4ebf11d344e" ns2:_="" ns3:_="">
     <xsd:import namespace="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
@@ -3223,25 +3217,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD9EFE20-B0BF-4817-AA37-C0305E12107B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D71E3CE6-3BAB-4EFC-B954-0CB76BF2E2C7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F56DC957-990F-47B2-AF0D-7029CF1F606B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3258,4 +3251,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D71E3CE6-3BAB-4EFC-B954-0CB76BF2E2C7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD9EFE20-B0BF-4817-AA37-C0305E12107B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>